<commit_message>
updates on the sys
</commit_message>
<xml_diff>
--- a/data/proveedor/drimel/listos/tiendaNube/drimel.xlsx
+++ b/data/proveedor/drimel/listos/tiendaNube/drimel.xlsx
@@ -422,7 +422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -430,7 +430,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="26" customWidth="1" min="1" max="1"/>
+    <col width="31" customWidth="1" min="1" max="1"/>
     <col width="10" customWidth="1" min="2" max="2"/>
     <col width="7" customWidth="1" min="3" max="3"/>
     <col width="22" customWidth="1" min="4" max="4"/>
@@ -461,17 +461,257 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
+          <t>PAMPERS-PREMIUM-MES-HP-XGx58</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>4895</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>5482</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>BABYSEC-ULTRA-REGULAR-Gx8</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>451</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>505</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>BABYSEC-ULTRA-REGULAR-Mx8</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>451</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>505</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>BABYSEC-ULTRA-REGULAR-XXGx8</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>451</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>505</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>BABYSEC-ULTRA-REGULAR-Px12</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>451</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>505</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>BABYSEC-ULTRA-REGULAR-XGx8</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>451</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>505</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>PAMPERS-PREMIUM-XTR-RN-x36</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>1950</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>2184</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
           <t>PAMPERS-PANTS-PC-MES-Gx64</t>
         </is>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B9" s="2" t="n">
         <v>5201</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C9" s="2" t="n">
         <v>5825</v>
       </c>
-      <c r="D2" s="2" t="n">
-        <v>5</v>
+      <c r="D9" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>PAMPERS-CONFORT-XTR-MES-XXGx54</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>4405</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>4934</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>PAMPERS-PREMIUM-XTR-MES-XXGx54</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>4895</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>5482</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>PAMPERS-CONFORT-XTR-HIPER-Px56</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>2501</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>2801</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>PAMPERS-SUPER-XTR-REG-Gx9</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>526</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>589</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>BABYSEC-PREMIUM-JUMBO-XGx48</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>3357</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>3760</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>BABYSEC-PREMIUM-JUMBO-XXGx44</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>3357</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>3760</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>BABYSEC-PREMIUM-JUMBO-Gx60</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>3357</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>3760</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>PAMPERS-TOTAL-PROTECT-XXGx34</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>2110</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>2363</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>